<commit_message>
why prop load so hard
</commit_message>
<xml_diff>
--- a/daq_system/inputs/CMS_Master_Data_Wiring_Dev6.xlsx
+++ b/daq_system/inputs/CMS_Master_Data_Wiring_Dev6.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nmaso\Documents\DAQ\PSPL_DAQ\daq_system\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1928B16-CBB7-406A-9253-4DC9779E68C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C59446F0-AB61-4DED-8ADB-46E4489D9CD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -187,15 +187,9 @@
     <t>TC-FU-202</t>
   </si>
   <si>
-    <t>TC-FU-BOTTOM</t>
-  </si>
-  <si>
     <t>Dev6/ai16</t>
   </si>
   <si>
-    <t>TC-FU-UPPER</t>
-  </si>
-  <si>
     <t>Dev6/ai17</t>
   </si>
   <si>
@@ -206,6 +200,12 @@
   </si>
   <si>
     <t>PoundsPerSquareInch</t>
+  </si>
+  <si>
+    <t>TC-FU-VENT</t>
+  </si>
+  <si>
+    <t>TC-BATTERY</t>
   </si>
 </sst>
 </file>
@@ -832,7 +832,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G7" sqref="G7"/>
+      <selection pane="topRight" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.265625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -898,7 +898,7 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A2" s="16" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>40</v>
@@ -971,7 +971,7 @@
         <v>47</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C4" s="18" t="s">
         <v>17</v>
@@ -1000,10 +1000,10 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A5" s="16" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C5" s="18" t="s">
         <v>17</v>
@@ -1032,16 +1032,16 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A6" s="16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C6" s="18" t="s">
         <v>17</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E6" s="18" t="s">
         <v>38</v>

</xml_diff>